<commit_message>
VERSIONE CON PID TUNATI IN CODE GEN BLOCKS
Sono state apportate modifiche anche a Parameters.m, ho provato a
correggere il segno dello yaw andando a mettere un + nella definizione
delle matrici in dynamic_tilt_matrici_TEST.
</commit_message>
<xml_diff>
--- a/Attitude identification/Risultati.xlsx
+++ b/Attitude identification/Risultati.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
     <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
+    <sheet name="Foglio4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="83">
   <si>
     <t>RBS_a_deltaTH1_290716</t>
   </si>
@@ -251,6 +252,30 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>PROVE GREY CON TIME DELAY</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>VAR A1</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>VAR B1</t>
+  </si>
+  <si>
+    <t>1/VAR A1</t>
+  </si>
+  <si>
+    <t>1/VAR B1</t>
+  </si>
+  <si>
+    <t>DEV STD</t>
   </si>
 </sst>
 </file>
@@ -865,11 +890,11 @@
         </c:dLbls>
         <c:gapWidth val="200"/>
         <c:overlap val="-80"/>
-        <c:axId val="1859498704"/>
-        <c:axId val="1859501968"/>
+        <c:axId val="2096469808"/>
+        <c:axId val="2096464368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1859498704"/>
+        <c:axId val="2096469808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -879,7 +904,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1859501968"/>
+        <c:crossAx val="2096464368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -887,7 +912,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1859501968"/>
+        <c:axId val="2096464368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0"/>
@@ -939,7 +964,7 @@
             <a:endParaRPr lang="it-CH"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1859498704"/>
+        <c:crossAx val="2096469808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1229,11 +1254,11 @@
         </c:dLbls>
         <c:gapWidth val="200"/>
         <c:overlap val="-80"/>
-        <c:axId val="1859497616"/>
-        <c:axId val="1859493808"/>
+        <c:axId val="2096468176"/>
+        <c:axId val="2096457840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1859497616"/>
+        <c:axId val="2096468176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1243,7 +1268,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1859493808"/>
+        <c:crossAx val="2096457840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1251,7 +1276,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1859493808"/>
+        <c:axId val="2096457840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1302,7 +1327,7 @@
             <a:endParaRPr lang="it-CH"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1859497616"/>
+        <c:crossAx val="2096468176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1592,11 +1617,11 @@
         </c:dLbls>
         <c:gapWidth val="200"/>
         <c:overlap val="-80"/>
-        <c:axId val="1859486736"/>
-        <c:axId val="1859493264"/>
+        <c:axId val="2096468720"/>
+        <c:axId val="2096460560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1859486736"/>
+        <c:axId val="2096468720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1606,7 +1631,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1859493264"/>
+        <c:crossAx val="2096460560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1614,7 +1639,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1859493264"/>
+        <c:axId val="2096460560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1665,7 +1690,7 @@
             <a:endParaRPr lang="it-CH"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1859486736"/>
+        <c:crossAx val="2096468720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1955,11 +1980,11 @@
         </c:dLbls>
         <c:gapWidth val="200"/>
         <c:overlap val="-80"/>
-        <c:axId val="1673974512"/>
-        <c:axId val="1673970704"/>
+        <c:axId val="2096470352"/>
+        <c:axId val="2096470896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1673974512"/>
+        <c:axId val="2096470352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1969,7 +1994,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1673970704"/>
+        <c:crossAx val="2096470896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1977,7 +2002,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1673970704"/>
+        <c:axId val="2096470896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2028,7 +2053,7 @@
             <a:endParaRPr lang="it-CH"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1673974512"/>
+        <c:crossAx val="2096470352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4686,8 +4711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4791,22 +4816,22 @@
         <v>0.156392</v>
       </c>
       <c r="G2" s="12">
-        <f>1/F2</f>
+        <f t="shared" ref="G2:G11" si="0">1/F2</f>
         <v>6.3941889610721772</v>
       </c>
       <c r="H2" s="12">
         <v>0.16152</v>
       </c>
       <c r="I2" s="12">
-        <f>1/H2</f>
+        <f t="shared" ref="I2:I11" si="1">1/H2</f>
         <v>6.1911837543338288</v>
       </c>
       <c r="J2" s="13">
-        <f>$B$41/E2</f>
+        <f t="shared" ref="J2:J11" si="2">$B$41/E2</f>
         <v>1.8370681106378726E-3</v>
       </c>
       <c r="K2" s="13">
-        <f>D2*$B$41</f>
+        <f t="shared" ref="K2:K11" si="3">D2*$B$41</f>
         <v>-3.5139140100000001E-2</v>
       </c>
       <c r="L2" s="12">
@@ -4816,25 +4841,25 @@
         <v>5.9208610000000004</v>
       </c>
       <c r="N2" s="13">
-        <f>$B$41/L2</f>
+        <f t="shared" ref="N2:N11" si="4">$B$41/L2</f>
         <v>1.3074012620103211E-3</v>
       </c>
       <c r="O2" s="13">
-        <f>-M2*N2</f>
+        <f t="shared" ref="O2:O11" si="5">-M2*N2</f>
         <v>-7.7409411435876924E-3</v>
       </c>
       <c r="P2" s="12">
         <v>3.0499999999999999E-4</v>
       </c>
       <c r="Q2" s="12">
-        <f>1/P2</f>
+        <f t="shared" ref="Q2:Q11" si="6">1/P2</f>
         <v>3278.688524590164</v>
       </c>
       <c r="R2" s="12">
         <v>2.9100000000000003E-4</v>
       </c>
       <c r="S2" s="12">
-        <f>1/R2</f>
+        <f t="shared" ref="S2:S11" si="7">1/R2</f>
         <v>3436.4261168384878</v>
       </c>
       <c r="T2" s="12">
@@ -4864,22 +4889,22 @@
         <v>0.15102099999999999</v>
       </c>
       <c r="G3" s="12">
-        <f>1/F3</f>
+        <f t="shared" si="0"/>
         <v>6.6215956721250695</v>
       </c>
       <c r="H3" s="12">
         <v>0.115693</v>
       </c>
       <c r="I3" s="12">
-        <f>1/H3</f>
+        <f t="shared" si="1"/>
         <v>8.6435652978140425</v>
       </c>
       <c r="J3" s="13">
-        <f>$B$41/E3</f>
+        <f t="shared" si="2"/>
         <v>1.8375544754620468E-3</v>
       </c>
       <c r="K3" s="13">
-        <f>D3*$B$41</f>
+        <f t="shared" si="3"/>
         <v>-3.8256414499999995E-2</v>
       </c>
       <c r="L3" s="12">
@@ -4889,25 +4914,25 @@
         <v>6.0501290000000001</v>
       </c>
       <c r="N3" s="13">
-        <f>$B$41/L3</f>
+        <f t="shared" si="4"/>
         <v>1.3351257720883272E-3</v>
       </c>
       <c r="O3" s="13">
-        <f>-M3*N3</f>
+        <f t="shared" si="5"/>
         <v>-8.07768315235898E-3</v>
       </c>
       <c r="P3" s="12">
         <v>3.3500000000000001E-4</v>
       </c>
       <c r="Q3" s="12">
-        <f>1/P3</f>
+        <f t="shared" si="6"/>
         <v>2985.0746268656717</v>
       </c>
       <c r="R3" s="12">
         <v>3.2499999999999999E-4</v>
       </c>
       <c r="S3" s="12">
-        <f>1/R3</f>
+        <f t="shared" si="7"/>
         <v>3076.9230769230771</v>
       </c>
       <c r="T3" s="12">
@@ -4934,22 +4959,22 @@
         <v>0.14516000000000001</v>
       </c>
       <c r="G4" s="12">
-        <f>1/F4</f>
+        <f t="shared" si="0"/>
         <v>6.8889501240011013</v>
       </c>
       <c r="H4" s="12">
         <v>0.12219099999999999</v>
       </c>
       <c r="I4" s="12">
-        <f>1/H4</f>
+        <f t="shared" si="1"/>
         <v>8.1839087985203491</v>
       </c>
       <c r="J4" s="13">
-        <f>$B$41/E4</f>
+        <f t="shared" si="2"/>
         <v>1.7654066005639017E-3</v>
       </c>
       <c r="K4" s="13">
-        <f>D4*$B$41</f>
+        <f t="shared" si="3"/>
         <v>-4.0564768100000002E-2</v>
       </c>
       <c r="L4" s="12">
@@ -4959,25 +4984,25 @@
         <v>7.037433</v>
       </c>
       <c r="N4" s="13">
-        <f>$B$41/L4</f>
+        <f t="shared" si="4"/>
         <v>1.2030815707993647E-3</v>
       </c>
       <c r="O4" s="13">
-        <f>-M4*N4</f>
+        <f t="shared" si="5"/>
         <v>-8.466605948035286E-3</v>
       </c>
       <c r="P4" s="12">
         <v>3.2499999999999999E-4</v>
       </c>
       <c r="Q4" s="12">
-        <f>1/P4</f>
+        <f t="shared" si="6"/>
         <v>3076.9230769230771</v>
       </c>
       <c r="R4" s="12">
         <v>3.28E-4</v>
       </c>
       <c r="S4" s="12">
-        <f>1/R4</f>
+        <f t="shared" si="7"/>
         <v>3048.7804878048778</v>
       </c>
       <c r="T4" s="12">
@@ -5004,22 +5029,22 @@
         <v>0.209928</v>
       </c>
       <c r="G5" s="12">
-        <f>1/F5</f>
+        <f t="shared" si="0"/>
         <v>4.763537974924736</v>
       </c>
       <c r="H5" s="12">
         <v>0.155025</v>
       </c>
       <c r="I5" s="12">
-        <f>1/H5</f>
+        <f t="shared" si="1"/>
         <v>6.450572488308338</v>
       </c>
       <c r="J5" s="13">
-        <f>$B$41/E5</f>
+        <f t="shared" si="2"/>
         <v>1.8149667799405643E-3</v>
       </c>
       <c r="K5" s="13">
-        <f>D5*$B$41</f>
+        <f t="shared" si="3"/>
         <v>-4.0893636800000001E-2</v>
       </c>
       <c r="L5" s="12">
@@ -5029,25 +5054,25 @@
         <v>6.5522679999999998</v>
       </c>
       <c r="N5" s="13">
-        <f>$B$41/L5</f>
+        <f t="shared" si="4"/>
         <v>1.2918783371694594E-3</v>
       </c>
       <c r="O5" s="13">
-        <f>-M5*N5</f>
+        <f t="shared" si="5"/>
         <v>-8.4647330885286587E-3</v>
       </c>
       <c r="P5" s="12">
         <v>3.7599999999999998E-4</v>
       </c>
       <c r="Q5" s="12">
-        <f>1/P5</f>
+        <f t="shared" si="6"/>
         <v>2659.5744680851067</v>
       </c>
       <c r="R5" s="12">
         <v>3.8499999999999998E-4</v>
       </c>
       <c r="S5" s="12">
-        <f>1/R5</f>
+        <f t="shared" si="7"/>
         <v>2597.4025974025976</v>
       </c>
       <c r="T5" s="12">
@@ -5074,22 +5099,22 @@
         <v>0.208125</v>
       </c>
       <c r="G6" s="12">
-        <f>1/F6</f>
+        <f t="shared" si="0"/>
         <v>4.8048048048048049</v>
       </c>
       <c r="H6" s="12">
         <v>0.16924500000000001</v>
       </c>
       <c r="I6" s="12">
-        <f>1/H6</f>
+        <f t="shared" si="1"/>
         <v>5.9085940500457914</v>
       </c>
       <c r="J6" s="13">
-        <f>$B$41/E6</f>
+        <f t="shared" si="2"/>
         <v>1.7673474157176897E-3</v>
       </c>
       <c r="K6" s="13">
-        <f>D6*$B$41</f>
+        <f t="shared" si="3"/>
         <v>-3.8749887500000003E-2</v>
       </c>
       <c r="L6" s="12">
@@ -5099,25 +5124,25 @@
         <v>6.6022759999999998</v>
       </c>
       <c r="N6" s="13">
-        <f>$B$41/L6</f>
+        <f t="shared" si="4"/>
         <v>1.2197543840992344E-3</v>
       </c>
       <c r="O6" s="13">
-        <f>-M6*N6</f>
+        <f t="shared" si="5"/>
         <v>-8.0531550960331565E-3</v>
       </c>
       <c r="P6" s="12">
         <v>3.97E-4</v>
       </c>
       <c r="Q6" s="12">
-        <f>1/P6</f>
+        <f t="shared" si="6"/>
         <v>2518.8916876574308</v>
       </c>
       <c r="R6" s="12">
         <v>3.9800000000000002E-4</v>
       </c>
       <c r="S6" s="12">
-        <f>1/R6</f>
+        <f t="shared" si="7"/>
         <v>2512.5628140703516</v>
       </c>
       <c r="T6" s="12">
@@ -5144,22 +5169,22 @@
         <v>0.30037599999999998</v>
       </c>
       <c r="G7" s="12">
-        <f>1/F7</f>
+        <f t="shared" si="0"/>
         <v>3.3291607851492797</v>
       </c>
       <c r="H7" s="12">
         <v>0.171379</v>
       </c>
       <c r="I7" s="12">
-        <f>1/H7</f>
+        <f t="shared" si="1"/>
         <v>5.8350206267979159</v>
       </c>
       <c r="J7" s="13">
-        <f>$B$41/E7</f>
+        <f t="shared" si="2"/>
         <v>1.7908502504930053E-3</v>
       </c>
       <c r="K7" s="13">
-        <f>D7*$B$41</f>
+        <f t="shared" si="3"/>
         <v>-4.21982142E-2</v>
       </c>
       <c r="L7" s="12">
@@ -5169,25 +5194,25 @@
         <v>7.97844</v>
       </c>
       <c r="N7" s="13">
-        <f>$B$41/L7</f>
+        <f t="shared" si="4"/>
         <v>1.1100765963628933E-3</v>
       </c>
       <c r="O7" s="13">
-        <f>-M7*N7</f>
+        <f t="shared" si="5"/>
         <v>-8.8566795194855632E-3</v>
       </c>
       <c r="P7" s="12">
         <v>4.4499999999999997E-4</v>
       </c>
       <c r="Q7" s="12">
-        <f>1/P7</f>
+        <f t="shared" si="6"/>
         <v>2247.1910112359551</v>
       </c>
       <c r="R7" s="12">
         <v>4.9600000000000002E-4</v>
       </c>
       <c r="S7" s="12">
-        <f>1/R7</f>
+        <f t="shared" si="7"/>
         <v>2016.1290322580644</v>
       </c>
       <c r="T7" s="12">
@@ -5214,22 +5239,22 @@
         <v>0.292018</v>
       </c>
       <c r="G8" s="12">
-        <f>1/F8</f>
+        <f t="shared" si="0"/>
         <v>3.4244464382332596</v>
       </c>
       <c r="H8" s="12">
         <v>0.20019700000000001</v>
       </c>
       <c r="I8" s="12">
-        <f>1/H8</f>
+        <f t="shared" si="1"/>
         <v>4.9950798463513433</v>
       </c>
       <c r="J8" s="13">
-        <f>$B$41/E8</f>
+        <f t="shared" si="2"/>
         <v>1.7691016604822537E-3</v>
       </c>
       <c r="K8" s="13">
-        <f>D8*$B$41</f>
+        <f t="shared" si="3"/>
         <v>-4.06442017E-2</v>
       </c>
       <c r="L8" s="12">
@@ -5239,25 +5264,25 @@
         <v>7.4341900000000001</v>
       </c>
       <c r="N8" s="13">
-        <f>$B$41/L8</f>
+        <f t="shared" si="4"/>
         <v>1.144782791358335E-3</v>
       </c>
       <c r="O8" s="13">
-        <f>-M8*N8</f>
+        <f t="shared" si="5"/>
         <v>-8.5105327796882197E-3</v>
       </c>
       <c r="P8" s="12">
         <v>4.5600000000000003E-4</v>
       </c>
       <c r="Q8" s="12">
-        <f>1/P8</f>
+        <f t="shared" si="6"/>
         <v>2192.9824561403507</v>
       </c>
       <c r="R8" s="12">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="S8" s="12">
-        <f>1/R8</f>
+        <f t="shared" si="7"/>
         <v>2000</v>
       </c>
       <c r="T8" s="12">
@@ -5284,22 +5309,22 @@
         <v>0.28787299999999999</v>
       </c>
       <c r="G9" s="12">
-        <f>1/F9</f>
+        <f t="shared" si="0"/>
         <v>3.4737540512656624</v>
       </c>
       <c r="H9" s="12">
         <v>0.19486800000000001</v>
       </c>
       <c r="I9" s="12">
-        <f>1/H9</f>
+        <f t="shared" si="1"/>
         <v>5.1316788800624007</v>
       </c>
       <c r="J9" s="13">
-        <f>$B$41/E9</f>
+        <f t="shared" si="2"/>
         <v>1.8114097357821483E-3</v>
       </c>
       <c r="K9" s="13">
-        <f>D9*$B$41</f>
+        <f t="shared" si="3"/>
         <v>-4.4798614E-2</v>
       </c>
       <c r="L9" s="12">
@@ -5309,25 +5334,25 @@
         <v>7.7598830000000003</v>
       </c>
       <c r="N9" s="13">
-        <f>$B$41/L9</f>
+        <f t="shared" si="4"/>
         <v>1.1860366409323583E-3</v>
       </c>
       <c r="O9" s="13">
-        <f>-M9*N9</f>
+        <f t="shared" si="5"/>
         <v>-9.2035055673481119E-3</v>
       </c>
       <c r="P9" s="12">
         <v>5.1099999999999995E-4</v>
       </c>
       <c r="Q9" s="12">
-        <f>1/P9</f>
+        <f t="shared" si="6"/>
         <v>1956.9471624266146</v>
       </c>
       <c r="R9" s="12">
         <v>5.7399999999999997E-4</v>
       </c>
       <c r="S9" s="12">
-        <f>1/R9</f>
+        <f t="shared" si="7"/>
         <v>1742.1602787456447</v>
       </c>
       <c r="T9" s="12">
@@ -5354,22 +5379,22 @@
         <v>0.38018999999999997</v>
       </c>
       <c r="G10" s="12">
-        <f>1/F10</f>
+        <f t="shared" si="0"/>
         <v>2.6302638154606908</v>
       </c>
       <c r="H10" s="12">
         <v>0.34822999999999998</v>
       </c>
       <c r="I10" s="12">
-        <f>1/H10</f>
+        <f t="shared" si="1"/>
         <v>2.8716652786951156</v>
       </c>
       <c r="J10" s="13">
-        <f>$B$41/E10</f>
+        <f t="shared" si="2"/>
         <v>1.8778041723714843E-3</v>
       </c>
       <c r="K10" s="13">
-        <f>D10*$B$41</f>
+        <f t="shared" si="3"/>
         <v>-3.9464099799999999E-2</v>
       </c>
       <c r="L10" s="12">
@@ -5379,25 +5404,25 @@
         <v>6.3025460000000004</v>
       </c>
       <c r="N10" s="13">
-        <f>$B$41/L10</f>
+        <f t="shared" si="4"/>
         <v>1.317305687819015E-3</v>
       </c>
       <c r="O10" s="13">
-        <f>-M10*N10</f>
+        <f t="shared" si="5"/>
         <v>-8.3023796935409819E-3</v>
       </c>
       <c r="P10" s="12">
         <v>5.9400000000000002E-4</v>
       </c>
       <c r="Q10" s="12">
-        <f>1/P10</f>
+        <f t="shared" si="6"/>
         <v>1683.5016835016834</v>
       </c>
       <c r="R10" s="12">
         <v>6.2500000000000001E-4</v>
       </c>
       <c r="S10" s="12">
-        <f>1/R10</f>
+        <f t="shared" si="7"/>
         <v>1600</v>
       </c>
       <c r="T10" s="12">
@@ -5427,22 +5452,22 @@
         <v>0.49456499999999998</v>
       </c>
       <c r="G11" s="12">
-        <f>1/F11</f>
+        <f t="shared" si="0"/>
         <v>2.0219789107599611</v>
       </c>
       <c r="H11" s="12">
         <v>0.24485699999999999</v>
       </c>
       <c r="I11" s="12">
-        <f>1/H11</f>
+        <f t="shared" si="1"/>
         <v>4.0840163850737374</v>
       </c>
       <c r="J11" s="13">
-        <f>$B$41/E11</f>
+        <f t="shared" si="2"/>
         <v>2.0474064032138316E-3</v>
       </c>
       <c r="K11" s="26">
-        <f>D11*$B$41</f>
+        <f t="shared" si="3"/>
         <v>-4.6719770000000001E-2</v>
       </c>
       <c r="L11" s="27">
@@ -5452,25 +5477,25 @@
         <v>9.2000779999999995</v>
       </c>
       <c r="N11" s="13">
-        <f>$B$41/L11</f>
+        <f t="shared" si="4"/>
         <v>1.101184767899117E-3</v>
       </c>
       <c r="O11" s="13">
-        <f>-M11*N11</f>
+        <f t="shared" si="5"/>
         <v>-1.0130985757083771E-2</v>
       </c>
       <c r="P11" s="12">
         <v>8.4099999999999995E-4</v>
       </c>
       <c r="Q11" s="12">
-        <f>1/P11</f>
+        <f t="shared" si="6"/>
         <v>1189.0606420927468</v>
       </c>
       <c r="R11" s="12">
         <v>1.0640000000000001E-3</v>
       </c>
       <c r="S11" s="12">
-        <f>1/R11</f>
+        <f t="shared" si="7"/>
         <v>939.84962406015029</v>
       </c>
       <c r="T11" s="12">
@@ -5541,7 +5566,7 @@
     </row>
     <row r="13" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="35" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="E13" s="32">
         <f>SQRT(1/G12)</f>
@@ -5659,22 +5684,22 @@
         <v>7.6746999999999996E-2</v>
       </c>
       <c r="G16" s="16">
-        <f>1/F16</f>
+        <f t="shared" ref="G16:G24" si="8">1/F16</f>
         <v>13.02982527004313</v>
       </c>
       <c r="H16" s="16">
         <v>7.0391999999999996E-2</v>
       </c>
       <c r="I16" s="12">
-        <f>1/H16</f>
+        <f t="shared" ref="I16:I24" si="9">1/H16</f>
         <v>14.206159790885328</v>
       </c>
       <c r="J16" s="17">
-        <f>$B$41/E16</f>
+        <f t="shared" ref="J16:J24" si="10">$B$41/E16</f>
         <v>1.9256428889653746E-3</v>
       </c>
       <c r="K16" s="17">
-        <f>D16*$B$41</f>
+        <f t="shared" ref="K16:K24" si="11">D16*$B$41</f>
         <v>-3.5169010100000002E-2</v>
       </c>
       <c r="L16" s="16">
@@ -5684,25 +5709,25 @@
         <v>5.2524959999999998</v>
       </c>
       <c r="N16" s="17">
-        <f>$B$41/L16</f>
+        <f t="shared" ref="N16:N24" si="12">$B$41/L16</f>
         <v>1.4745979036371744E-3</v>
       </c>
       <c r="O16" s="17">
-        <f>-M16*N16</f>
+        <f t="shared" ref="O16:O24" si="13">-M16*N16</f>
         <v>-7.7453195904626437E-3</v>
       </c>
       <c r="P16" s="16">
         <v>2.1000000000000001E-4</v>
       </c>
       <c r="Q16" s="16">
-        <f>1/P16</f>
+        <f t="shared" ref="Q16:Q24" si="14">1/P16</f>
         <v>4761.9047619047615</v>
       </c>
       <c r="R16" s="16">
         <v>1.92E-4</v>
       </c>
       <c r="S16" s="25">
-        <f>1/R16</f>
+        <f t="shared" ref="S16:S24" si="15">1/R16</f>
         <v>5208.333333333333</v>
       </c>
       <c r="T16" s="18">
@@ -5729,22 +5754,22 @@
         <v>0.11065</v>
       </c>
       <c r="G17" s="16">
-        <f>1/F17</f>
+        <f t="shared" si="8"/>
         <v>9.0375056484410301</v>
       </c>
       <c r="H17" s="12">
         <v>0.10102899999999999</v>
       </c>
       <c r="I17" s="12">
-        <f>1/H17</f>
+        <f t="shared" si="9"/>
         <v>9.8981480564986288</v>
       </c>
       <c r="J17" s="13">
-        <f>$B$41/E17</f>
+        <f t="shared" si="10"/>
         <v>1.9025636213580684E-3</v>
       </c>
       <c r="K17" s="13">
-        <f>D17*$B$41</f>
+        <f t="shared" si="11"/>
         <v>-3.7089486300000002E-2</v>
       </c>
       <c r="L17" s="12">
@@ -5754,25 +5779,25 @@
         <v>5.2807789999999999</v>
       </c>
       <c r="N17" s="13">
-        <f>$B$41/L17</f>
+        <f t="shared" si="12"/>
         <v>1.488886617814803E-3</v>
       </c>
       <c r="O17" s="13">
-        <f>-M17*N17</f>
+        <f t="shared" si="13"/>
         <v>-7.8624811847374382E-3</v>
       </c>
       <c r="P17" s="12">
         <v>2.5300000000000002E-4</v>
       </c>
       <c r="Q17" s="16">
-        <f>1/P17</f>
+        <f t="shared" si="14"/>
         <v>3952.569169960474</v>
       </c>
       <c r="R17" s="12">
         <v>2.3599999999999999E-4</v>
       </c>
       <c r="S17" s="25">
-        <f>1/R17</f>
+        <f t="shared" si="15"/>
         <v>4237.2881355932204</v>
       </c>
       <c r="T17" s="20">
@@ -5799,22 +5824,22 @@
         <v>0.117627</v>
       </c>
       <c r="G18" s="16">
-        <f>1/F18</f>
+        <f t="shared" si="8"/>
         <v>8.5014494971392622</v>
       </c>
       <c r="H18" s="12">
         <v>0.100815</v>
       </c>
       <c r="I18" s="12">
-        <f>1/H18</f>
+        <f t="shared" si="9"/>
         <v>9.9191588553290675</v>
       </c>
       <c r="J18" s="13">
-        <f>$B$41/E18</f>
+        <f t="shared" si="10"/>
         <v>1.9418866843133261E-3</v>
       </c>
       <c r="K18" s="13">
-        <f>D18*$B$41</f>
+        <f t="shared" si="11"/>
         <v>-3.8014117300000004E-2</v>
       </c>
       <c r="L18" s="12">
@@ -5824,25 +5849,25 @@
         <v>6.0085860000000002</v>
       </c>
       <c r="N18" s="13">
-        <f>$B$41/L18</f>
+        <f t="shared" si="12"/>
         <v>1.4086814714074588E-3</v>
       </c>
       <c r="O18" s="13">
-        <f>-M18*N18</f>
+        <f t="shared" si="13"/>
         <v>-8.4641837675582584E-3</v>
       </c>
       <c r="P18" s="12">
         <v>2.6200000000000003E-4</v>
       </c>
       <c r="Q18" s="16">
-        <f>1/P18</f>
+        <f t="shared" si="14"/>
         <v>3816.7938931297708</v>
       </c>
       <c r="R18" s="12">
         <v>2.61E-4</v>
       </c>
       <c r="S18" s="25">
-        <f>1/R18</f>
+        <f t="shared" si="15"/>
         <v>3831.4176245210729</v>
       </c>
       <c r="T18" s="20">
@@ -5869,22 +5894,22 @@
         <v>0.21015200000000001</v>
       </c>
       <c r="G19" s="16">
-        <f>1/F19</f>
+        <f t="shared" si="8"/>
         <v>4.7584605428451789</v>
       </c>
       <c r="H19" s="12">
         <v>0.169706</v>
       </c>
       <c r="I19" s="12">
-        <f>1/H19</f>
+        <f t="shared" si="9"/>
         <v>5.8925435753597402</v>
       </c>
       <c r="J19" s="13">
-        <f>$B$41/E19</f>
+        <f t="shared" si="10"/>
         <v>1.8935988636936062E-3</v>
       </c>
       <c r="K19" s="13">
-        <f>D19*$B$41</f>
+        <f t="shared" si="11"/>
         <v>-4.0592609000000002E-2</v>
       </c>
       <c r="L19" s="12">
@@ -5894,25 +5919,25 @@
         <v>6.4942840000000004</v>
       </c>
       <c r="N19" s="13">
-        <f>$B$41/L19</f>
+        <f t="shared" si="12"/>
         <v>1.3239624215761142E-3</v>
       </c>
       <c r="O19" s="13">
-        <f>-M19*N19</f>
+        <f t="shared" si="13"/>
         <v>-8.5981879710430135E-3</v>
       </c>
       <c r="P19" s="12">
         <v>3.4699999999999998E-4</v>
       </c>
       <c r="Q19" s="16">
-        <f>1/P19</f>
+        <f t="shared" si="14"/>
         <v>2881.8443804034582</v>
       </c>
       <c r="R19" s="12">
         <v>3.5599999999999998E-4</v>
       </c>
       <c r="S19" s="25">
-        <f>1/R19</f>
+        <f t="shared" si="15"/>
         <v>2808.9887640449438</v>
       </c>
       <c r="T19" s="20">
@@ -5939,22 +5964,22 @@
         <v>0.18825500000000001</v>
       </c>
       <c r="G20" s="16">
-        <f>1/F20</f>
+        <f t="shared" si="8"/>
         <v>5.3119439058723534</v>
       </c>
       <c r="H20" s="12">
         <v>0.14266400000000001</v>
       </c>
       <c r="I20" s="12">
-        <f>1/H20</f>
+        <f t="shared" si="9"/>
         <v>7.0094768126507034</v>
       </c>
       <c r="J20" s="13">
-        <f>$B$41/E20</f>
+        <f t="shared" si="10"/>
         <v>1.9505654746123488E-3</v>
       </c>
       <c r="K20" s="13">
-        <f>D20*$B$41</f>
+        <f t="shared" si="11"/>
         <v>-4.0719577100000001E-2</v>
       </c>
       <c r="L20" s="12">
@@ -5964,25 +5989,25 @@
         <v>6.6029090000000004</v>
       </c>
       <c r="N20" s="13">
-        <f>$B$41/L20</f>
+        <f t="shared" si="12"/>
         <v>1.3403056990058575E-3</v>
       </c>
       <c r="O20" s="13">
-        <f>-M20*N20</f>
+        <f t="shared" si="13"/>
         <v>-8.8499165627170685E-3</v>
       </c>
       <c r="P20" s="12">
         <v>3.3100000000000002E-4</v>
       </c>
       <c r="Q20" s="16">
-        <f>1/P20</f>
+        <f t="shared" si="14"/>
         <v>3021.1480362537764</v>
       </c>
       <c r="R20" s="12">
         <v>3.4699999999999998E-4</v>
       </c>
       <c r="S20" s="25">
-        <f>1/R20</f>
+        <f t="shared" si="15"/>
         <v>2881.8443804034582</v>
       </c>
       <c r="T20" s="20">
@@ -6012,22 +6037,22 @@
         <v>0.35119299999999998</v>
       </c>
       <c r="G21" s="16">
-        <f>1/F21</f>
+        <f t="shared" si="8"/>
         <v>2.8474371641803797</v>
       </c>
       <c r="H21" s="12">
         <v>0.252189</v>
       </c>
       <c r="I21" s="12">
-        <f>1/H21</f>
+        <f t="shared" si="9"/>
         <v>3.9652800082477824</v>
       </c>
       <c r="J21" s="13">
-        <f>$B$41/E21</f>
+        <f t="shared" si="10"/>
         <v>1.8393172454384931E-3</v>
       </c>
       <c r="K21" s="13">
-        <f>D21*$B$41</f>
+        <f t="shared" si="11"/>
         <v>-4.9366540400000006E-2</v>
       </c>
       <c r="L21" s="12">
@@ -6037,25 +6062,25 @@
         <v>7.0448940000000002</v>
       </c>
       <c r="N21" s="13">
-        <f>$B$41/L21</f>
+        <f t="shared" si="12"/>
         <v>1.3538793506847212E-3</v>
       </c>
       <c r="O21" s="13">
-        <f>-M21*N21</f>
+        <f t="shared" si="13"/>
         <v>-9.5379365143626882E-3</v>
       </c>
       <c r="P21" s="12">
         <v>4.8000000000000001E-4</v>
       </c>
       <c r="Q21" s="16">
-        <f>1/P21</f>
+        <f t="shared" si="14"/>
         <v>2083.3333333333335</v>
       </c>
       <c r="R21" s="12">
         <v>5.44E-4</v>
       </c>
       <c r="S21" s="25">
-        <f>1/R21</f>
+        <f t="shared" si="15"/>
         <v>1838.2352941176471</v>
       </c>
       <c r="T21" s="20">
@@ -6085,22 +6110,22 @@
         <v>0.31247599999999998</v>
       </c>
       <c r="G22" s="16">
-        <f>1/F22</f>
+        <f t="shared" si="8"/>
         <v>3.2002457788758178</v>
       </c>
       <c r="H22" s="12">
         <v>0.228185</v>
       </c>
       <c r="I22" s="12">
-        <f>1/H22</f>
+        <f t="shared" si="9"/>
         <v>4.3824090102329247</v>
       </c>
       <c r="J22" s="13">
-        <f>$B$41/E22</f>
+        <f t="shared" si="10"/>
         <v>1.9396578104653012E-3</v>
       </c>
       <c r="K22" s="13">
-        <f>D22*$B$41</f>
+        <f t="shared" si="11"/>
         <v>-4.6260668099999999E-2</v>
       </c>
       <c r="L22" s="12">
@@ -6110,25 +6135,25 @@
         <v>6.592155</v>
       </c>
       <c r="N22" s="13">
-        <f>$B$41/L22</f>
+        <f t="shared" si="12"/>
         <v>1.4280239863663916E-3</v>
       </c>
       <c r="O22" s="13">
-        <f>-M22*N22</f>
+        <f t="shared" si="13"/>
         <v>-9.4137554618451396E-3</v>
       </c>
       <c r="P22" s="12">
         <v>4.6099999999999998E-4</v>
       </c>
       <c r="Q22" s="16">
-        <f>1/P22</f>
+        <f t="shared" si="14"/>
         <v>2169.1973969631235</v>
       </c>
       <c r="R22" s="12">
         <v>5.2599999999999999E-4</v>
       </c>
       <c r="S22" s="25">
-        <f>1/R22</f>
+        <f t="shared" si="15"/>
         <v>1901.1406844106464</v>
       </c>
       <c r="T22" s="20">
@@ -6158,22 +6183,22 @@
         <v>0.25424799999999997</v>
       </c>
       <c r="G23" s="16">
-        <f>1/F23</f>
+        <f t="shared" si="8"/>
         <v>3.9331676158711182</v>
       </c>
       <c r="H23" s="12">
         <v>0.154753</v>
       </c>
       <c r="I23" s="12">
-        <f>1/H23</f>
+        <f t="shared" si="9"/>
         <v>6.4619102699139921</v>
       </c>
       <c r="J23" s="13">
-        <f>$B$41/E23</f>
+        <f t="shared" si="10"/>
         <v>1.9314427821326917E-3</v>
       </c>
       <c r="K23" s="13">
-        <f>D23*$B$41</f>
+        <f t="shared" si="11"/>
         <v>-4.1210701699999998E-2</v>
       </c>
       <c r="L23" s="12">
@@ -6183,25 +6208,25 @@
         <v>6.9114690000000003</v>
       </c>
       <c r="N23" s="13">
-        <f>$B$41/L23</f>
+        <f t="shared" si="12"/>
         <v>1.3172800800906289E-3</v>
       </c>
       <c r="O23" s="13">
-        <f>-M23*N23</f>
+        <f t="shared" si="13"/>
         <v>-9.1043404378638986E-3</v>
       </c>
       <c r="P23" s="12">
         <v>4.2900000000000002E-4</v>
       </c>
       <c r="Q23" s="16">
-        <f>1/P23</f>
+        <f t="shared" si="14"/>
         <v>2331.0023310023307</v>
       </c>
       <c r="R23" s="12">
         <v>5.04E-4</v>
       </c>
       <c r="S23" s="25">
-        <f>1/R23</f>
+        <f t="shared" si="15"/>
         <v>1984.1269841269841</v>
       </c>
       <c r="T23" s="20">
@@ -6231,22 +6256,22 @@
         <v>0.302066</v>
       </c>
       <c r="G24" s="16">
-        <f>1/F24</f>
+        <f t="shared" si="8"/>
         <v>3.3105347837889734</v>
       </c>
       <c r="H24" s="22">
         <v>0.20593</v>
       </c>
       <c r="I24" s="22">
-        <f>1/H24</f>
+        <f t="shared" si="9"/>
         <v>4.8560190355946196</v>
       </c>
       <c r="J24" s="23">
-        <f>$B$41/E24</f>
+        <f t="shared" si="10"/>
         <v>1.9247555140040915E-3</v>
       </c>
       <c r="K24" s="23">
-        <f>D24*$B$41</f>
+        <f t="shared" si="11"/>
         <v>-4.6316246900000003E-2</v>
       </c>
       <c r="L24" s="22">
@@ -6256,25 +6281,25 @@
         <v>4.438377</v>
       </c>
       <c r="N24" s="23">
-        <f>$B$41/L24</f>
+        <f t="shared" si="12"/>
         <v>1.9364090778857569E-3</v>
       </c>
       <c r="O24" s="23">
-        <f>-M24*N24</f>
+        <f t="shared" si="13"/>
         <v>-8.5945135138793521E-3</v>
       </c>
       <c r="P24" s="22">
         <v>5.8699999999999996E-4</v>
       </c>
       <c r="Q24" s="16">
-        <f>1/P24</f>
+        <f t="shared" si="14"/>
         <v>1703.5775127768316</v>
       </c>
       <c r="R24" s="22">
         <v>6.4000000000000005E-4</v>
       </c>
       <c r="S24" s="25">
-        <f>1/R24</f>
+        <f t="shared" si="15"/>
         <v>1562.4999999999998</v>
       </c>
       <c r="T24" s="24">
@@ -6338,7 +6363,7 @@
     </row>
     <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D26" s="35" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="E26" s="32">
         <f>SQRT(1/G25)</f>
@@ -6467,11 +6492,11 @@
         <v>0.9995182322120737</v>
       </c>
       <c r="J29" s="17">
-        <f>$B$41/E29</f>
+        <f t="shared" ref="J29:J38" si="16">$B$41/E29</f>
         <v>1.5645568035891845E-3</v>
       </c>
       <c r="K29" s="17">
-        <f>D29*$B$41</f>
+        <f t="shared" ref="K29:K38" si="17">D29*$B$41</f>
         <v>-3.8497321200000004E-2</v>
       </c>
       <c r="L29" s="16">
@@ -6481,11 +6506,11 @@
         <v>6.6093039999999998</v>
       </c>
       <c r="N29" s="17">
-        <f>$B$41/L29</f>
+        <f t="shared" ref="N29:N38" si="18">$B$41/L29</f>
         <v>1.0851978278764564E-3</v>
       </c>
       <c r="O29" s="17">
-        <f>-M29*N29</f>
+        <f t="shared" ref="O29:O38" si="19">-M29*N29</f>
         <v>-7.1724023445751744E-3</v>
       </c>
       <c r="P29" s="16">
@@ -6526,22 +6551,22 @@
         <v>0.32664799999999999</v>
       </c>
       <c r="G30" s="16">
-        <f t="shared" ref="G30:G38" si="0">1/F30</f>
+        <f t="shared" ref="G30:G38" si="20">1/F30</f>
         <v>3.0613994269060272</v>
       </c>
       <c r="H30" s="12">
         <v>0.38941500000000001</v>
       </c>
       <c r="I30" s="12">
-        <f t="shared" ref="I30:I38" si="1">1/H30</f>
+        <f t="shared" ref="I30:I38" si="21">1/H30</f>
         <v>2.5679544958463336</v>
       </c>
       <c r="J30" s="13">
-        <f>$B$41/E30</f>
+        <f t="shared" si="16"/>
         <v>1.576865937613672E-3</v>
       </c>
       <c r="K30" s="13">
-        <f>D30*$B$41</f>
+        <f t="shared" si="17"/>
         <v>-3.4892331500000005E-2</v>
       </c>
       <c r="L30" s="12">
@@ -6551,25 +6576,25 @@
         <v>6.9196920000000004</v>
       </c>
       <c r="N30" s="13">
-        <f>$B$41/L30</f>
+        <f t="shared" si="18"/>
         <v>1.0481528544713031E-3</v>
       </c>
       <c r="O30" s="13">
-        <f>-M30*N30</f>
+        <f t="shared" si="19"/>
         <v>-7.2528949218622404E-3</v>
       </c>
       <c r="P30" s="12">
         <v>6.2E-4</v>
       </c>
       <c r="Q30" s="16">
-        <f t="shared" ref="Q30:Q38" si="2">1/P30</f>
+        <f t="shared" ref="Q30:Q38" si="22">1/P30</f>
         <v>1612.9032258064517</v>
       </c>
       <c r="R30" s="12">
         <v>6.2E-4</v>
       </c>
       <c r="S30" s="25">
-        <f t="shared" ref="S30:S38" si="3">1/R30</f>
+        <f t="shared" ref="S30:S38" si="23">1/R30</f>
         <v>1612.9032258064517</v>
       </c>
       <c r="T30" s="20">
@@ -6599,22 +6624,22 @@
         <v>0.40225899999999998</v>
       </c>
       <c r="G31" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="20"/>
         <v>2.4859605378624221</v>
       </c>
       <c r="H31" s="12">
         <v>0.46753600000000001</v>
       </c>
       <c r="I31" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="21"/>
         <v>2.1388727285171623</v>
       </c>
       <c r="J31" s="13">
-        <f>$B$41/E31</f>
+        <f t="shared" si="16"/>
         <v>1.5681440816872135E-3</v>
       </c>
       <c r="K31" s="13">
-        <f>D31*$B$41</f>
+        <f t="shared" si="17"/>
         <v>-4.0284690499999998E-2</v>
       </c>
       <c r="L31" s="12">
@@ -6624,25 +6649,25 @@
         <v>6.9562660000000003</v>
       </c>
       <c r="N31" s="13">
-        <f>$B$41/L31</f>
+        <f t="shared" si="18"/>
         <v>1.0940430946761526E-3</v>
       </c>
       <c r="O31" s="13">
-        <f>-M31*N31</f>
+        <f t="shared" si="19"/>
         <v>-7.610454782030502E-3</v>
       </c>
       <c r="P31" s="12">
         <v>6.3400000000000001E-4</v>
       </c>
       <c r="Q31" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="22"/>
         <v>1577.2870662460568</v>
       </c>
       <c r="R31" s="12">
         <v>6.1600000000000001E-4</v>
       </c>
       <c r="S31" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="23"/>
         <v>1623.3766233766235</v>
       </c>
       <c r="T31" s="20">
@@ -6669,22 +6694,22 @@
         <v>0.42220999999999997</v>
       </c>
       <c r="G32" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="20"/>
         <v>2.368489614173042</v>
       </c>
       <c r="H32" s="12">
         <v>0.41877199999999998</v>
       </c>
       <c r="I32" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="21"/>
         <v>2.3879342458426067</v>
       </c>
       <c r="J32" s="13">
-        <f>$B$41/E32</f>
+        <f t="shared" si="16"/>
         <v>1.7322392084440439E-3</v>
       </c>
       <c r="K32" s="13">
-        <f>D32*$B$41</f>
+        <f t="shared" si="17"/>
         <v>-4.2690873500000004E-2</v>
       </c>
       <c r="L32" s="12">
@@ -6694,25 +6719,25 @@
         <v>7.7647919999999999</v>
       </c>
       <c r="N32" s="13">
-        <f>$B$41/L32</f>
+        <f t="shared" si="18"/>
         <v>1.117666156808345E-3</v>
       </c>
       <c r="O32" s="13">
-        <f>-M32*N32</f>
+        <f t="shared" si="19"/>
         <v>-8.6784452330561819E-3</v>
       </c>
       <c r="P32" s="12">
         <v>6.0099999999999997E-4</v>
       </c>
       <c r="Q32" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="22"/>
         <v>1663.893510815308</v>
       </c>
       <c r="R32" s="12">
         <v>6.2799999999999998E-4</v>
       </c>
       <c r="S32" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="23"/>
         <v>1592.3566878980891</v>
       </c>
       <c r="T32" s="20">
@@ -6739,22 +6764,22 @@
         <v>0.25467699999999999</v>
       </c>
       <c r="G33" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="20"/>
         <v>3.9265422476313137</v>
       </c>
       <c r="H33" s="12">
         <v>0.260743</v>
       </c>
       <c r="I33" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="21"/>
         <v>3.835194041642537</v>
       </c>
       <c r="J33" s="13">
-        <f>$B$41/E33</f>
+        <f t="shared" si="16"/>
         <v>1.6528076869999455E-3</v>
       </c>
       <c r="K33" s="13">
-        <f>D33*$B$41</f>
+        <f t="shared" si="17"/>
         <v>-3.6868087800000005E-2</v>
       </c>
       <c r="L33" s="12">
@@ -6764,25 +6789,25 @@
         <v>7.212199</v>
       </c>
       <c r="N33" s="13">
-        <f>$B$41/L33</f>
+        <f t="shared" si="18"/>
         <v>1.0976561205358567E-3</v>
       </c>
       <c r="O33" s="13">
-        <f>-M33*N33</f>
+        <f t="shared" si="19"/>
         <v>-7.9165143748725856E-3</v>
       </c>
       <c r="P33" s="12">
         <v>4.8700000000000002E-4</v>
       </c>
       <c r="Q33" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="22"/>
         <v>2053.3880903490758</v>
       </c>
       <c r="R33" s="12">
         <v>4.8000000000000001E-4</v>
       </c>
       <c r="S33" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="23"/>
         <v>2083.3333333333335</v>
       </c>
       <c r="T33" s="20">
@@ -6809,22 +6834,22 @@
         <v>0.28028399999999998</v>
       </c>
       <c r="G34" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="20"/>
         <v>3.56780979292432</v>
       </c>
       <c r="H34" s="12">
         <v>0.28211599999999998</v>
       </c>
       <c r="I34" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="21"/>
         <v>3.5446412114165806</v>
       </c>
       <c r="J34" s="13">
-        <f>$B$41/E34</f>
+        <f t="shared" si="16"/>
         <v>1.7099065511168262E-3</v>
       </c>
       <c r="K34" s="13">
-        <f>D34*$B$41</f>
+        <f t="shared" si="17"/>
         <v>-3.6443727799999999E-2</v>
       </c>
       <c r="L34" s="12">
@@ -6834,25 +6859,25 @@
         <v>6.0895200000000003</v>
       </c>
       <c r="N34" s="13">
-        <f>$B$41/L34</f>
+        <f t="shared" si="18"/>
         <v>1.2058163429322949E-3</v>
       </c>
       <c r="O34" s="13">
-        <f>-M34*N34</f>
+        <f t="shared" si="19"/>
         <v>-7.3428427366130688E-3</v>
       </c>
       <c r="P34" s="12">
         <v>5.4699999999999996E-4</v>
       </c>
       <c r="Q34" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="22"/>
         <v>1828.1535648994518</v>
       </c>
       <c r="R34" s="12">
         <v>4.8799999999999999E-4</v>
       </c>
       <c r="S34" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="23"/>
         <v>2049.1803278688526</v>
       </c>
       <c r="T34" s="20">
@@ -6879,22 +6904,22 @@
         <v>0.61662799999999995</v>
       </c>
       <c r="G35" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="20"/>
         <v>1.6217233080560729</v>
       </c>
       <c r="H35" s="12">
         <v>0.51230900000000001</v>
       </c>
       <c r="I35" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="21"/>
         <v>1.9519469695047325</v>
       </c>
       <c r="J35" s="13">
-        <f>$B$41/E35</f>
+        <f t="shared" si="16"/>
         <v>1.8661553521788451E-3</v>
       </c>
       <c r="K35" s="13">
-        <f>D35*$B$41</f>
+        <f t="shared" si="17"/>
         <v>-4.0347705900000003E-2</v>
       </c>
       <c r="L35" s="12">
@@ -6904,25 +6929,25 @@
         <v>8.4252210000000005</v>
       </c>
       <c r="N35" s="13">
-        <f>$B$41/L35</f>
+        <f t="shared" si="18"/>
         <v>1.0789104638393207E-3</v>
       </c>
       <c r="O35" s="13">
-        <f>-M35*N35</f>
+        <f t="shared" si="19"/>
         <v>-9.0900590970587856E-3</v>
       </c>
       <c r="P35" s="12">
         <v>7.2900000000000005E-4</v>
       </c>
       <c r="Q35" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="22"/>
         <v>1371.7421124828531</v>
       </c>
       <c r="R35" s="12">
         <v>8.1899999999999996E-4</v>
       </c>
       <c r="S35" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="23"/>
         <v>1221.001221001221</v>
       </c>
       <c r="T35" s="20">
@@ -6949,22 +6974,22 @@
         <v>0.59106899999999996</v>
       </c>
       <c r="G36" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="20"/>
         <v>1.6918498517093605</v>
       </c>
       <c r="H36" s="12">
         <v>0.51750200000000002</v>
       </c>
       <c r="I36" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="21"/>
         <v>1.9323596817017132</v>
       </c>
       <c r="J36" s="13">
-        <f>$B$41/E36</f>
+        <f t="shared" si="16"/>
         <v>1.6974193458014002E-3</v>
       </c>
       <c r="K36" s="13">
-        <f>D36*$B$41</f>
+        <f t="shared" si="17"/>
         <v>-4.3839642799999995E-2</v>
       </c>
       <c r="L36" s="12">
@@ -6974,25 +6999,25 @@
         <v>8.2087559999999993</v>
       </c>
       <c r="N36" s="13">
-        <f>$B$41/L36</f>
+        <f t="shared" si="18"/>
         <v>1.0545554286107441E-3</v>
       </c>
       <c r="O36" s="13">
-        <f>-M36*N36</f>
+        <f t="shared" si="19"/>
         <v>-8.6565882019410158E-3</v>
       </c>
       <c r="P36" s="12">
         <v>6.7900000000000002E-4</v>
       </c>
       <c r="Q36" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="22"/>
         <v>1472.7540500736377</v>
       </c>
       <c r="R36" s="12">
         <v>7.3999999999999999E-4</v>
       </c>
       <c r="S36" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="23"/>
         <v>1351.3513513513515</v>
       </c>
       <c r="T36" s="20">
@@ -7019,22 +7044,22 @@
         <v>1.1026370000000001</v>
       </c>
       <c r="G37" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="20"/>
         <v>0.90691678222297989</v>
       </c>
       <c r="H37" s="12">
         <v>1.2831379999999999</v>
       </c>
       <c r="I37" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="21"/>
         <v>0.77933940075034802</v>
       </c>
       <c r="J37" s="13">
-        <f>$B$41/E37</f>
+        <f t="shared" si="16"/>
         <v>1.778813058491173E-3</v>
       </c>
       <c r="K37" s="13">
-        <f>D37*$B$41</f>
+        <f t="shared" si="17"/>
         <v>-4.11042821E-2</v>
       </c>
       <c r="L37" s="12">
@@ -7044,25 +7069,25 @@
         <v>7.6513419999999996</v>
       </c>
       <c r="N37" s="13">
-        <f>$B$41/L37</f>
+        <f t="shared" si="18"/>
         <v>1.1379954243745142E-3</v>
       </c>
       <c r="O37" s="13">
-        <f>-M37*N37</f>
+        <f t="shared" si="19"/>
         <v>-8.7071921863245434E-3</v>
       </c>
       <c r="P37" s="12">
         <v>6.4899999999999995E-4</v>
       </c>
       <c r="Q37" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="22"/>
         <v>1540.8320493066258</v>
       </c>
       <c r="R37" s="12">
         <v>6.9399999999999996E-4</v>
       </c>
       <c r="S37" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="23"/>
         <v>1440.9221902017291</v>
       </c>
       <c r="T37" s="20">
@@ -7089,22 +7114,22 @@
         <v>0.50985000000000003</v>
       </c>
       <c r="G38" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="20"/>
         <v>1.9613611846621555</v>
       </c>
       <c r="H38" s="22">
         <v>0.49577399999999999</v>
       </c>
       <c r="I38" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="21"/>
         <v>2.0170480904605728</v>
       </c>
       <c r="J38" s="23">
-        <f>$B$41/E38</f>
+        <f t="shared" si="16"/>
         <v>1.7033310043451479E-3</v>
       </c>
       <c r="K38" s="23">
-        <f>D38*$B$41</f>
+        <f t="shared" si="17"/>
         <v>-4.31956353E-2</v>
       </c>
       <c r="L38" s="22">
@@ -7114,25 +7139,25 @@
         <v>7.6723590000000002</v>
       </c>
       <c r="N38" s="23">
-        <f>$B$41/L38</f>
+        <f t="shared" si="18"/>
         <v>1.090456315737709E-3</v>
       </c>
       <c r="O38" s="23">
-        <f>-M38*N38</f>
+        <f t="shared" si="19"/>
         <v>-8.366372328157054E-3</v>
       </c>
       <c r="P38" s="22">
         <v>7.1599999999999995E-4</v>
       </c>
       <c r="Q38" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="22"/>
         <v>1396.6480446927376</v>
       </c>
       <c r="R38" s="22">
         <v>7.3200000000000001E-4</v>
       </c>
       <c r="S38" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="23"/>
         <v>1366.1202185792349</v>
       </c>
       <c r="T38" s="24">
@@ -7193,7 +7218,7 @@
     </row>
     <row r="40" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D40" s="35" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="E40" s="32">
         <f>SQRT(1/G39)</f>
@@ -7696,4 +7721,359 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>-7.252802</v>
+      </c>
+      <c r="C4">
+        <v>1.0492980000000001</v>
+      </c>
+      <c r="D4">
+        <v>7.5615600000000001</v>
+      </c>
+      <c r="E4">
+        <v>0.41426400000000002</v>
+      </c>
+      <c r="F4">
+        <f>1/C4</f>
+        <v>0.95301811306225681</v>
+      </c>
+      <c r="G4">
+        <f>1/E4</f>
+        <v>2.4139196261321283</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>-6.3322859999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.24972900000000001</v>
+      </c>
+      <c r="D5">
+        <v>8.4937229999999992</v>
+      </c>
+      <c r="E5">
+        <v>0.139903</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F13" si="0">1/C5</f>
+        <v>4.0043407053245721</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G13" si="1">1/E5</f>
+        <v>7.1478095537622499</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>-7.3257899999999996</v>
+      </c>
+      <c r="C6">
+        <v>0.68346700000000005</v>
+      </c>
+      <c r="D6">
+        <v>8.3476959999999991</v>
+      </c>
+      <c r="E6">
+        <v>0.37683800000000001</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>1.4631284319506281</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>2.6536601935049013</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>-6.0062439999999997</v>
+      </c>
+      <c r="C7">
+        <v>0.40074399999999999</v>
+      </c>
+      <c r="D7">
+        <v>7.3630019999999998</v>
+      </c>
+      <c r="E7">
+        <v>0.20460600000000001</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>2.4953586329427266</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>4.8874422059959137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>-6.586741</v>
+      </c>
+      <c r="C8">
+        <v>0.25804300000000002</v>
+      </c>
+      <c r="D8">
+        <v>8.3818940000000008</v>
+      </c>
+      <c r="E8">
+        <v>0.15476100000000001</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>3.8753231050638846</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>6.4615762369072307</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>-7.1971080000000001</v>
+      </c>
+      <c r="C9">
+        <v>0.45514500000000002</v>
+      </c>
+      <c r="D9">
+        <v>8.9825870000000005</v>
+      </c>
+      <c r="E9">
+        <v>0.24515000000000001</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>2.1971020224324116</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>4.0791352233326537</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>-6.6846350000000001</v>
+      </c>
+      <c r="C10">
+        <v>0.27104</v>
+      </c>
+      <c r="D10">
+        <v>8.9606680000000001</v>
+      </c>
+      <c r="E10">
+        <v>0.163435</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>3.6894923258559622</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>6.1186404380946557</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>-6.9999969999999996</v>
+      </c>
+      <c r="C11">
+        <v>0.65954599999999997</v>
+      </c>
+      <c r="D11">
+        <v>8.0606810000000007</v>
+      </c>
+      <c r="E11">
+        <v>0.38256899999999999</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>1.5161944731679065</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>2.6139075565453553</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>-6.5396830000000001</v>
+      </c>
+      <c r="C12">
+        <v>0.979765</v>
+      </c>
+      <c r="D12">
+        <v>7.5830609999999998</v>
+      </c>
+      <c r="E12">
+        <v>0.42071399999999998</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>1.0206529116675938</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>2.3769116311793761</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>-5.7791709999999998</v>
+      </c>
+      <c r="C13">
+        <v>0.17050100000000001</v>
+      </c>
+      <c r="D13">
+        <v>8.0261359999999993</v>
+      </c>
+      <c r="E13">
+        <v>0.12400700000000001</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>5.8650682400689726</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>8.0640608997879148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f>SUM(F4:F13)</f>
+        <v>27.079678961536914</v>
+      </c>
+      <c r="G14">
+        <f>SUM(G4:G13)</f>
+        <v>46.817063565242378</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18">
+        <f>SUMPRODUCT(B4:B13,F4:F13)/F14</f>
+        <v>-6.4683101365676894</v>
+      </c>
+      <c r="F18">
+        <f>SUMPRODUCT(D4:D13,G4:G13)/G14</f>
+        <v>8.2565758814413908</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19">
+        <f>1/F14</f>
+        <v>3.6928059650203654E-2</v>
+      </c>
+      <c r="F19">
+        <f>1/G14</f>
+        <v>2.1359733478509179E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20">
+        <f>SQRT(E19)</f>
+        <v>0.19216674959577074</v>
+      </c>
+      <c r="F20">
+        <f>SQRT(F19)</f>
+        <v>0.14614969544446263</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>